<commit_message>
replace normal with 8x8 block medium
</commit_message>
<xml_diff>
--- a/figures/c1b_IS3/result3.xlsx
+++ b/figures/c1b_IS3/result3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\sakakibara\monte-carlo-ray-tracer_approx\figures\c1b_IS3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB2EE1A9-0DA1-41FD-ACE7-07A1B883EB36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C85677A-F918-4035-9703-36E9B1EE10A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="4" r:id="rId1"/>
@@ -816,6 +816,19 @@
               <a:rPr lang="en-US" altLang="ja-JP"/>
               <a:t>MSE</a:t>
             </a:r>
+            <a:r>
+              <a:rPr lang="ja-JP" altLang="en-US"/>
+              <a:t>（</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" altLang="ja-JP"/>
+              <a:t>water_caustics</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="ja-JP" altLang="en-US"/>
+              <a:t>）</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" altLang="ja-JP"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -1154,6 +1167,7 @@
         <c:axId val="1120664479"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:min val="135"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -4554,6 +4568,19 @@
               <a:rPr lang="en-US" altLang="ja-JP"/>
               <a:t>MSE</a:t>
             </a:r>
+            <a:r>
+              <a:rPr lang="ja-JP" altLang="en-US"/>
+              <a:t>（</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" altLang="ja-JP"/>
+              <a:t>hexagon_room</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="ja-JP" altLang="en-US"/>
+              <a:t>）</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" altLang="ja-JP"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -11706,7 +11733,7 @@
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18.75"/>
+  <sheetFormatPr defaultRowHeight="17.649999999999999"/>
   <cols>
     <col min="1" max="1" width="9" customWidth="1"/>
   </cols>
@@ -11948,7 +11975,7 @@
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18.75"/>
+  <sheetFormatPr defaultRowHeight="17.649999999999999"/>
   <cols>
     <col min="1" max="1" width="9" customWidth="1"/>
   </cols>
@@ -12190,7 +12217,7 @@
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18.75"/>
+  <sheetFormatPr defaultRowHeight="17.649999999999999"/>
   <cols>
     <col min="1" max="1" width="9" customWidth="1"/>
   </cols>
@@ -12385,10 +12412,10 @@
   <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4:E14"/>
+      <selection activeCell="P21" sqref="P21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18.75"/>
+  <sheetFormatPr defaultRowHeight="17.649999999999999"/>
   <cols>
     <col min="1" max="1" width="9" customWidth="1"/>
   </cols>
@@ -12626,11 +12653,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81994667-F05C-4EE5-A3F4-656FFA2CF137}">
   <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="R18" sqref="R18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18.75"/>
+  <sheetFormatPr defaultRowHeight="17.649999999999999"/>
   <cols>
     <col min="1" max="1" width="9" customWidth="1"/>
   </cols>

</xml_diff>